<commit_message>
Deployed 909fff3 with MkDocs version: 1.5.3
</commit_message>
<xml_diff>
--- a/assets/images/Planilha_Importação.xlsx
+++ b/assets/images/Planilha_Importação.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinicius\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482737EE-5BC8-4EF9-82EA-03AFAA66FA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676478E0-78B8-458D-AA25-C7C71E686014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
     <t>Código do Produto</t>
   </si>
   <si>
-    <t>Quantidade</t>
-  </si>
-  <si>
     <t>CapCP1</t>
   </si>
   <si>
@@ -509,13 +506,16 @@
   </si>
   <si>
     <t>Refil Proteina Vegetal Caramelo Machiatto Muke | 900g | +Mu</t>
+  </si>
+  <si>
+    <t>Preencher Quantidade Aqui</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -536,8 +536,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,6 +553,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
@@ -563,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,6 +597,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,13 +822,13 @@
   <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -821,651 +836,651 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>